<commit_message>
feat: added VerifyAndFixNumberOfSentMessages, and included PR Review remarks
</commit_message>
<xml_diff>
--- a/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData-plusNewMedium.xlsx
+++ b/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData-plusNewMedium.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance.SnapshotCreator.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA24FFF-D68B-4B4F-B47B-5A80F25DED41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71050466-76F7-4453-BD40-61BD0E0126BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="38355" windowHeight="7980" tabRatio="259" activeTab="1" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="259" activeTab="2" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="heavy" sheetId="1" r:id="rId1"/>
@@ -308,11 +308,8 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -348,6 +345,13 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -688,7 +692,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,492 +724,492 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="T1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="15">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
         <v>5000</v>
       </c>
-      <c r="E2" s="15">
-        <v>0</v>
-      </c>
-      <c r="F2" s="15">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="15">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="15">
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14">
         <v>50</v>
       </c>
-      <c r="O2" s="15">
-        <v>1</v>
-      </c>
-      <c r="P2" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="12">
+      <c r="O2" s="14">
+        <v>1</v>
+      </c>
+      <c r="P2" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11">
         <f>na1_*ma1_+na2_*ma2_+na3_*ma3_</f>
         <v>780000</v>
       </c>
-      <c r="R2" s="12">
+      <c r="R2" s="11">
         <f>na1_*I3+na2_*I4+na3_*I5</f>
         <v>780000</v>
       </c>
-      <c r="S2" s="14">
+      <c r="S2" s="13">
         <f>U2-R2</f>
         <v>1000</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="11">
         <f>na1_*ra1_+na2_*ra2_+na3_*ra3_</f>
         <v>21000</v>
       </c>
-      <c r="U2" s="12">
+      <c r="U2" s="11">
         <f>nc1_*mc1_+nc2_*mc2_+nc3_*mc3_</f>
         <v>781000</v>
       </c>
-      <c r="V2" s="12">
+      <c r="V2" s="11">
         <f>nc1_*I6+nc2_*I7+nc3_*I8</f>
         <v>780000</v>
       </c>
-      <c r="W2" s="14">
+      <c r="W2" s="13">
         <f>Q2-V2</f>
         <v>0</v>
       </c>
-      <c r="X2" s="12">
+      <c r="X2" s="11">
         <f>nc1_*rc_1+nc2_*rc_2+nc3_*rc_3</f>
         <v>21000</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>500</v>
       </c>
-      <c r="E3" s="15">
-        <v>1</v>
-      </c>
-      <c r="F3" s="15">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="15">
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14">
         <f>10+K3</f>
         <v>10</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na1_)*M3)+L3</f>
         <v>15</v>
       </c>
-      <c r="J3" s="21" t="str">
+      <c r="J3" s="20" t="str">
         <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
         <v/>
       </c>
-      <c r="K3" s="20">
-        <v>0</v>
-      </c>
-      <c r="L3" s="20">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8">
+      <c r="K3" s="19">
+        <v>0</v>
+      </c>
+      <c r="L3" s="19">
+        <v>0</v>
+      </c>
+      <c r="M3" s="24">
         <v>0.01</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="14">
         <v>50</v>
       </c>
-      <c r="O3" s="15">
-        <v>1</v>
-      </c>
-      <c r="P3" s="16">
+      <c r="O3" s="14">
+        <v>1</v>
+      </c>
+      <c r="P3" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>1500</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>2</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>2</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="15">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
         <f>50+K4</f>
         <v>50</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na2_)*M4)+L4</f>
         <v>130</v>
       </c>
-      <c r="J4" s="21" t="str">
+      <c r="J4" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="20">
-        <v>0</v>
-      </c>
-      <c r="L4" s="20">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8">
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19">
+        <v>0</v>
+      </c>
+      <c r="M4" s="24">
         <v>0.25</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="14">
         <v>500</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="14">
         <v>2</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>3500</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>5</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>5</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="15">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
         <f>200+K5</f>
         <v>200</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na3_)*M5)+L5</f>
         <v>165</v>
       </c>
-      <c r="J5" s="21" t="str">
+      <c r="J5" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="20">
-        <v>0</v>
-      </c>
-      <c r="L5" s="20">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8">
+      <c r="K5" s="19">
+        <v>0</v>
+      </c>
+      <c r="L5" s="19">
+        <v>0</v>
+      </c>
+      <c r="M5" s="24">
         <v>0.74</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="14">
         <v>1500</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="14">
         <v>3</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="15">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>10</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>100</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc1_)*G6)</f>
         <v>21</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="22">
         <v>0.01</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <f>100+K6</f>
         <v>100</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc1_)*M6)+L6</f>
         <v>780</v>
       </c>
-      <c r="J6" s="21" t="str">
+      <c r="J6" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K6" s="20">
-        <v>0</v>
-      </c>
-      <c r="L6" s="20">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8">
+      <c r="K6" s="19">
+        <v>0</v>
+      </c>
+      <c r="L6" s="19">
+        <v>0</v>
+      </c>
+      <c r="M6" s="24">
         <v>0.01</v>
       </c>
-      <c r="N6" s="15">
-        <v>0</v>
-      </c>
-      <c r="O6" s="15">
-        <v>1</v>
-      </c>
-      <c r="P6" s="16">
+      <c r="N6" s="14">
+        <v>0</v>
+      </c>
+      <c r="O6" s="14">
+        <v>1</v>
+      </c>
+      <c r="P6" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>20</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>8000</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc2_)*G7)</f>
         <v>252</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="23">
         <v>0.24</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <f>12000+K7</f>
         <v>12000</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc2_)*M7)+L7</f>
         <v>9360</v>
       </c>
-      <c r="J7" s="21" t="str">
+      <c r="J7" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="20">
-        <v>0</v>
-      </c>
-      <c r="L7" s="20">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8">
+      <c r="K7" s="19">
+        <v>0</v>
+      </c>
+      <c r="L7" s="19">
+        <v>0</v>
+      </c>
+      <c r="M7" s="24">
         <v>0.24</v>
       </c>
-      <c r="N7" s="15">
-        <v>0</v>
-      </c>
-      <c r="O7" s="15">
-        <v>1</v>
-      </c>
-      <c r="P7" s="16">
+      <c r="N7" s="14">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <v>1</v>
+      </c>
+      <c r="P7" s="15">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>30</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>12000</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc3_)*G8)</f>
         <v>525</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="23">
         <v>0.75</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <f>18000+K8</f>
         <v>18000</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc3_)*M8)+L8</f>
         <v>19500</v>
       </c>
-      <c r="J8" s="21" t="str">
+      <c r="J8" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="20">
-        <v>0</v>
-      </c>
-      <c r="L8" s="20">
-        <v>0</v>
-      </c>
-      <c r="M8" s="8">
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0</v>
+      </c>
+      <c r="M8" s="24">
         <v>0.75</v>
       </c>
-      <c r="N8" s="15">
-        <v>0</v>
-      </c>
-      <c r="O8" s="15">
-        <v>1</v>
-      </c>
-      <c r="P8" s="16">
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <v>1</v>
+      </c>
+      <c r="P8" s="15">
         <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1217,10 +1221,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72308825-AF3B-4E77-8452-3E1DA88E9FFD}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,489 +1256,489 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="T1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="15">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
         <v>2500</v>
       </c>
-      <c r="E2" s="15">
-        <v>0</v>
-      </c>
-      <c r="F2" s="15">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="15">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="15">
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14">
         <v>25</v>
       </c>
-      <c r="O2" s="15">
-        <v>1</v>
-      </c>
-      <c r="P2" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="12">
+      <c r="O2" s="14">
+        <v>1</v>
+      </c>
+      <c r="P2" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11">
         <f>D3*H3+D4*H4+D5*H5</f>
         <v>195000</v>
       </c>
-      <c r="R2" s="17">
+      <c r="R2" s="16">
         <f>D3*I3+D4*I4+D5*I5</f>
         <v>194000</v>
       </c>
-      <c r="S2" s="18">
+      <c r="S2" s="17">
         <f>U2-R2</f>
         <v>1250</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="11">
         <f>D3*F3+D4*F4+D5*F5</f>
         <v>4500</v>
       </c>
-      <c r="U2" s="12">
+      <c r="U2" s="11">
         <f>D6*H6+D7*H7+D8*H8</f>
         <v>195250</v>
       </c>
-      <c r="V2" s="17">
+      <c r="V2" s="16">
         <f>D6*I6+D7*I7+D8*I8</f>
         <v>195000</v>
       </c>
-      <c r="W2" s="14">
+      <c r="W2" s="13">
         <f>Q2-V2</f>
         <v>0</v>
       </c>
-      <c r="X2" s="12">
+      <c r="X2" s="11">
         <f>D6*F6+D7*F7+D8*F8</f>
         <v>4500</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>250</v>
       </c>
-      <c r="E3" s="15">
-        <v>1</v>
-      </c>
-      <c r="F3" s="15">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="15">
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14">
         <v>5</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D3)*M3)+L3</f>
         <v>7</v>
       </c>
-      <c r="J3" s="21" t="str">
+      <c r="J3" s="20" t="str">
         <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
         <v/>
       </c>
-      <c r="K3" s="20">
-        <v>0</v>
-      </c>
-      <c r="L3" s="20">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8">
+      <c r="K3" s="19">
+        <v>0</v>
+      </c>
+      <c r="L3" s="19">
+        <v>0</v>
+      </c>
+      <c r="M3" s="24">
         <v>0.01</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="14">
         <v>25</v>
       </c>
-      <c r="O3" s="15">
-        <v>1</v>
-      </c>
-      <c r="P3" s="16">
+      <c r="O3" s="14">
+        <v>1</v>
+      </c>
+      <c r="P3" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>750</v>
       </c>
-      <c r="E4" s="15">
-        <v>1</v>
-      </c>
-      <c r="F4" s="15">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="15">
+      <c r="E4" s="14">
+        <v>1</v>
+      </c>
+      <c r="F4" s="14">
+        <v>1</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
         <v>25</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D4)*M4)+L4</f>
         <v>65</v>
       </c>
-      <c r="J4" s="21" t="str">
+      <c r="J4" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="20">
-        <v>0</v>
-      </c>
-      <c r="L4" s="20">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8">
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19">
+        <v>0</v>
+      </c>
+      <c r="M4" s="24">
         <v>0.25</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="14">
         <v>250</v>
       </c>
-      <c r="O4" s="15">
-        <v>1</v>
-      </c>
-      <c r="P4" s="16">
+      <c r="O4" s="14">
+        <v>1</v>
+      </c>
+      <c r="P4" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>1750</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>2</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>2</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="15">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
         <v>100</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D5)*M5)+L5</f>
         <v>82</v>
       </c>
-      <c r="J5" s="21" t="str">
+      <c r="J5" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="20">
-        <v>0</v>
-      </c>
-      <c r="L5" s="20">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8">
+      <c r="K5" s="19">
+        <v>0</v>
+      </c>
+      <c r="L5" s="19">
+        <v>0</v>
+      </c>
+      <c r="M5" s="24">
         <v>0.74</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="14">
         <v>750</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="14">
         <v>2</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>5</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>50</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*G6)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="22">
         <v>0.01</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>50</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D6)*M6)+L6</f>
         <v>390</v>
       </c>
-      <c r="J6" s="21" t="str">
+      <c r="J6" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K6" s="20">
-        <v>0</v>
-      </c>
-      <c r="L6" s="20">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8">
+      <c r="K6" s="19">
+        <v>0</v>
+      </c>
+      <c r="L6" s="19">
+        <v>0</v>
+      </c>
+      <c r="M6" s="24">
         <v>0.01</v>
       </c>
-      <c r="N6" s="15">
-        <v>0</v>
-      </c>
-      <c r="O6" s="15">
-        <v>1</v>
-      </c>
-      <c r="P6" s="16">
+      <c r="N6" s="14">
+        <v>0</v>
+      </c>
+      <c r="O6" s="14">
+        <v>1</v>
+      </c>
+      <c r="P6" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>10</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>4000</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*G7)</f>
         <v>108</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="22">
         <v>0.24</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>6000</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D7)*M7)+L7</f>
         <v>4680</v>
       </c>
-      <c r="J7" s="21" t="str">
+      <c r="J7" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="20">
-        <v>0</v>
-      </c>
-      <c r="L7" s="20">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8">
+      <c r="K7" s="19">
+        <v>0</v>
+      </c>
+      <c r="L7" s="19">
+        <v>0</v>
+      </c>
+      <c r="M7" s="24">
         <v>0.24</v>
       </c>
-      <c r="N7" s="15">
-        <v>0</v>
-      </c>
-      <c r="O7" s="15">
-        <v>1</v>
-      </c>
-      <c r="P7" s="16">
+      <c r="N7" s="14">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <v>1</v>
+      </c>
+      <c r="P7" s="15">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>15</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>6000</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*G8)</f>
         <v>225</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="22">
         <v>0.75</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>9000</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D8)*M8)+L8</f>
         <v>9750</v>
       </c>
-      <c r="J8" s="21" t="str">
+      <c r="J8" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="20">
-        <v>0</v>
-      </c>
-      <c r="L8" s="20">
-        <v>0</v>
-      </c>
-      <c r="M8" s="8">
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0</v>
+      </c>
+      <c r="M8" s="24">
         <v>0.75</v>
       </c>
-      <c r="N8" s="15">
-        <v>0</v>
-      </c>
-      <c r="O8" s="15">
-        <v>1</v>
-      </c>
-      <c r="P8" s="16">
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <v>1</v>
+      </c>
+      <c r="P8" s="15">
         <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="19"/>
+      <c r="F11" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1746,10 +1750,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E26EECF-D978-410A-A017-B2DC302577D6}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,495 +1785,495 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="T1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="15">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
         <v>10</v>
       </c>
-      <c r="E2" s="15">
-        <v>0</v>
-      </c>
-      <c r="F2" s="15">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="15">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="15">
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14">
         <v>50</v>
       </c>
-      <c r="O2" s="15">
-        <v>1</v>
-      </c>
-      <c r="P2" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="12">
+      <c r="O2" s="14">
+        <v>1</v>
+      </c>
+      <c r="P2" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11">
         <f>D3*H3+D4*H4+D5*H5</f>
         <v>16500</v>
       </c>
-      <c r="R2" s="17">
+      <c r="R2" s="16">
         <f>D3*I3+D4*I4+D5*I5</f>
         <v>16500</v>
       </c>
-      <c r="S2" s="18">
+      <c r="S2" s="17">
         <f>U2-R2</f>
         <v>0</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="11">
         <f>D3*F3+D4*F4+D5*F5</f>
         <v>1800</v>
       </c>
-      <c r="U2" s="12">
+      <c r="U2" s="11">
         <f>D6*H6+D7*H7+D8*H8</f>
         <v>16500</v>
       </c>
-      <c r="V2" s="17">
+      <c r="V2" s="16">
         <f>D6*I6+D7*I7+D8*I8</f>
         <v>16499</v>
       </c>
-      <c r="W2" s="14">
+      <c r="W2" s="13">
         <f>Q2-V2</f>
         <v>1</v>
       </c>
-      <c r="X2" s="12">
+      <c r="X2" s="11">
         <f>D6*F6+D7*F7+D8*F8</f>
         <v>1803</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>50</v>
       </c>
-      <c r="E3" s="15">
-        <v>0</v>
-      </c>
-      <c r="F3" s="15">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="15">
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14">
         <f>0+K3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D3)*M3)+L3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="21" t="str">
+      <c r="J3" s="20" t="str">
         <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
         <v>Messages must be 0 on 0 Relationships</v>
       </c>
-      <c r="K3" s="20">
-        <v>0</v>
-      </c>
-      <c r="L3" s="20">
+      <c r="K3" s="19">
+        <v>0</v>
+      </c>
+      <c r="L3" s="19">
         <v>-3</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="24">
         <v>0.01</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="14">
         <v>5</v>
       </c>
-      <c r="O3" s="15">
-        <v>1</v>
-      </c>
-      <c r="P3" s="16">
+      <c r="O3" s="14">
+        <v>1</v>
+      </c>
+      <c r="P3" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>150</v>
       </c>
-      <c r="E4" s="15">
-        <v>0</v>
-      </c>
-      <c r="F4" s="15">
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
         <v>2</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="15">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14">
         <f>10+K4</f>
         <v>10</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D4)*M4)+L4</f>
         <v>30</v>
       </c>
-      <c r="J4" s="21" t="str">
+      <c r="J4" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="20">
-        <v>0</v>
-      </c>
-      <c r="L4" s="20">
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19">
         <v>3</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="24">
         <v>0.25</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="14">
         <v>60</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="14">
         <v>2</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>300</v>
       </c>
-      <c r="E5" s="15">
-        <v>0</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
         <v>5</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="15">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
         <f>50+K5</f>
         <v>50</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D5)*M5)+L5</f>
         <v>40</v>
       </c>
-      <c r="J5" s="21" t="str">
+      <c r="J5" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="20">
-        <v>0</v>
-      </c>
-      <c r="L5" s="20">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8">
+      <c r="K5" s="19">
+        <v>0</v>
+      </c>
+      <c r="L5" s="19">
+        <v>0</v>
+      </c>
+      <c r="M5" s="24">
         <v>0.74</v>
       </c>
-      <c r="N5" s="15">
-        <v>1</v>
-      </c>
-      <c r="O5" s="15">
+      <c r="N5" s="14">
+        <v>1</v>
+      </c>
+      <c r="O5" s="14">
         <v>3</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="15">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>2</v>
       </c>
-      <c r="E6" s="15">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*G6)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="22">
         <v>0.01</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <f>0+K6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D6)*M6)+L6</f>
         <v>82</v>
       </c>
-      <c r="J6" s="21" t="str">
+      <c r="J6" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K6" s="20">
-        <v>0</v>
-      </c>
-      <c r="L6" s="20">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8">
+      <c r="K6" s="19">
+        <v>0</v>
+      </c>
+      <c r="L6" s="19">
+        <v>0</v>
+      </c>
+      <c r="M6" s="24">
         <v>0.01</v>
       </c>
-      <c r="N6" s="15">
-        <v>0</v>
-      </c>
-      <c r="O6" s="15">
-        <v>1</v>
-      </c>
-      <c r="P6" s="16">
+      <c r="N6" s="14">
+        <v>0</v>
+      </c>
+      <c r="O6" s="14">
+        <v>1</v>
+      </c>
+      <c r="P6" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>15</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>20</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*G7)</f>
         <v>29</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="22">
         <v>0.24</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <f>440+K7</f>
         <v>440</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D7)*M7)+L7</f>
         <v>264</v>
       </c>
-      <c r="J7" s="21" t="str">
+      <c r="J7" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="20">
-        <v>0</v>
-      </c>
-      <c r="L7" s="20">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8">
+      <c r="K7" s="19">
+        <v>0</v>
+      </c>
+      <c r="L7" s="19">
+        <v>0</v>
+      </c>
+      <c r="M7" s="24">
         <v>0.24</v>
       </c>
-      <c r="N7" s="15">
-        <v>0</v>
-      </c>
-      <c r="O7" s="15">
-        <v>1</v>
-      </c>
-      <c r="P7" s="16">
+      <c r="N7" s="14">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <v>1</v>
+      </c>
+      <c r="P7" s="15">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>15</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>30</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*G8)</f>
         <v>90</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="22">
         <v>0.75</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <f>660+K8</f>
         <v>660</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D8)*M8)+L8</f>
         <v>825</v>
       </c>
-      <c r="J8" s="21" t="str">
+      <c r="J8" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="20">
-        <v>0</v>
-      </c>
-      <c r="L8" s="20">
-        <v>0</v>
-      </c>
-      <c r="M8" s="8">
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0</v>
+      </c>
+      <c r="M8" s="24">
         <v>0.75</v>
       </c>
-      <c r="N8" s="15">
-        <v>0</v>
-      </c>
-      <c r="O8" s="15">
-        <v>1</v>
-      </c>
-      <c r="P8" s="16">
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <v>1</v>
+      </c>
+      <c r="P8" s="15">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="19"/>
+      <c r="F11" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2315,494 +2319,494 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="S1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="T1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="15">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
         <v>5</v>
       </c>
-      <c r="E2" s="15">
-        <v>0</v>
-      </c>
-      <c r="F2" s="15">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="15">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="15">
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="14">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="14">
         <v>50</v>
       </c>
-      <c r="O2" s="15">
-        <v>1</v>
-      </c>
-      <c r="P2" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="12">
+      <c r="O2" s="14">
+        <v>1</v>
+      </c>
+      <c r="P2" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11">
         <f>D3*H3+D4*H4+D5*H5</f>
         <v>48</v>
       </c>
-      <c r="R2" s="17">
+      <c r="R2" s="16">
         <f>D3*I3+D4*I4+D5*I5</f>
         <v>45</v>
       </c>
-      <c r="S2" s="18">
+      <c r="S2" s="17">
         <f>U2-R2</f>
         <v>3</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="11">
         <f>D3*F3+D4*F4+D5*F5</f>
         <v>22</v>
       </c>
-      <c r="U2" s="12">
+      <c r="U2" s="11">
         <f>D6*H6+D7*H7+D8*H8</f>
         <v>48</v>
       </c>
-      <c r="V2" s="17">
+      <c r="V2" s="16">
         <f>D6*I6+D7*I7+D8*I8</f>
         <v>46</v>
       </c>
-      <c r="W2" s="14">
+      <c r="W2" s="13">
         <f>Q2-V2</f>
         <v>2</v>
       </c>
-      <c r="X2" s="12">
+      <c r="X2" s="11">
         <f>D6*F6+D7*F7+D8*F8</f>
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15">
-        <v>1</v>
-      </c>
-      <c r="E3" s="15">
-        <v>0</v>
-      </c>
-      <c r="F3" s="15">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="15">
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="14">
         <f>0+K3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D3)*M3)+L3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="21" t="str">
+      <c r="J3" s="20" t="str">
         <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
         <v/>
       </c>
-      <c r="K3" s="20">
-        <v>0</v>
-      </c>
-      <c r="L3" s="20">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8">
+      <c r="K3" s="19">
+        <v>0</v>
+      </c>
+      <c r="L3" s="19">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
         <v>0.01</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="14">
         <v>50</v>
       </c>
-      <c r="O3" s="15">
-        <v>1</v>
-      </c>
-      <c r="P3" s="16">
+      <c r="O3" s="14">
+        <v>1</v>
+      </c>
+      <c r="P3" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>3</v>
       </c>
-      <c r="E4" s="15">
-        <v>0</v>
-      </c>
-      <c r="F4" s="15">
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
         <v>2</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="15">
+      <c r="G4" s="5"/>
+      <c r="H4" s="14">
         <f>4+K4</f>
         <v>4</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D4)*M4)+L4</f>
         <v>4</v>
       </c>
-      <c r="J4" s="21" t="str">
+      <c r="J4" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="20">
-        <v>0</v>
-      </c>
-      <c r="L4" s="20">
-        <v>0</v>
-      </c>
-      <c r="M4" s="8">
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
         <v>0.25</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="14">
         <v>60</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="14">
         <v>2</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="15">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>3</v>
       </c>
-      <c r="E5" s="15">
-        <v>0</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
         <v>5</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="15">
+      <c r="G5" s="5"/>
+      <c r="H5" s="14">
         <f>12+K5</f>
         <v>12</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D5)*M5)+L5</f>
         <v>11</v>
       </c>
-      <c r="J5" s="21" t="str">
+      <c r="J5" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="20">
-        <v>0</v>
-      </c>
-      <c r="L5" s="20">
-        <v>0</v>
-      </c>
-      <c r="M5" s="8">
+      <c r="K5" s="19">
+        <v>0</v>
+      </c>
+      <c r="L5" s="19">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
         <v>0.74</v>
       </c>
-      <c r="N5" s="15">
-        <v>1</v>
-      </c>
-      <c r="O5" s="15">
+      <c r="N5" s="14">
+        <v>1</v>
+      </c>
+      <c r="O5" s="14">
         <v>3</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="15">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15">
-        <v>1</v>
-      </c>
-      <c r="E6" s="15">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*G6)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>0.01</v>
       </c>
-      <c r="H6" s="15">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D6)*M6)+L6</f>
         <v>0</v>
       </c>
-      <c r="J6" s="21" t="str">
+      <c r="J6" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K6" s="20">
-        <v>0</v>
-      </c>
-      <c r="L6" s="20">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8">
+      <c r="K6" s="19">
+        <v>0</v>
+      </c>
+      <c r="L6" s="19">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
         <v>0.01</v>
       </c>
-      <c r="N6" s="15">
-        <v>0</v>
-      </c>
-      <c r="O6" s="15">
-        <v>1</v>
-      </c>
-      <c r="P6" s="16">
+      <c r="N6" s="14">
+        <v>0</v>
+      </c>
+      <c r="O6" s="14">
+        <v>1</v>
+      </c>
+      <c r="P6" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>20</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*G7)</f>
         <v>3</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>0.24</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <f>8+K7</f>
         <v>8</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D7)*M7)+L7</f>
         <v>5</v>
       </c>
-      <c r="J7" s="21" t="str">
+      <c r="J7" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="20">
-        <v>0</v>
-      </c>
-      <c r="L7" s="20">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8">
+      <c r="K7" s="19">
+        <v>0</v>
+      </c>
+      <c r="L7" s="19">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
         <v>0.24</v>
       </c>
-      <c r="N7" s="15">
-        <v>0</v>
-      </c>
-      <c r="O7" s="15">
-        <v>1</v>
-      </c>
-      <c r="P7" s="16">
+      <c r="N7" s="14">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <v>1</v>
+      </c>
+      <c r="P7" s="15">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>4</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>30</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*G8)</f>
         <v>5</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>0.75</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <f>8+K8</f>
         <v>8</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D8)*M8)+L8</f>
         <v>9</v>
       </c>
-      <c r="J8" s="21" t="str">
+      <c r="J8" s="20" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="20">
-        <v>0</v>
-      </c>
-      <c r="L8" s="20">
-        <v>0</v>
-      </c>
-      <c r="M8" s="8">
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
         <v>0.75</v>
       </c>
-      <c r="N8" s="15">
-        <v>0</v>
-      </c>
-      <c r="O8" s="15">
-        <v>1</v>
-      </c>
-      <c r="P8" s="16">
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <v>1</v>
+      </c>
+      <c r="P8" s="15">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="19"/>
+      <c r="F11" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: heavy loadtest data corrected according to confluence Performance Test Data.xls
</commit_message>
<xml_diff>
--- a/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData-plusNewMedium.xlsx
+++ b/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData-plusNewMedium.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance.SnapshotCreator.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71050466-76F7-4453-BD40-61BD0E0126BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2507222C-6902-400D-9D53-8E556D7558DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="259" activeTab="2" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
+    <workbookView xWindow="5175" yWindow="270" windowWidth="28740" windowHeight="14580" tabRatio="259" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="heavy" sheetId="1" r:id="rId1"/>
@@ -690,9 +690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B50230-BD5E-4064-AF79-EFC0F2FDB528}">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,11 +842,11 @@
       </c>
       <c r="R2" s="11">
         <f>na1_*I3+na2_*I4+na3_*I5</f>
-        <v>780000</v>
+        <v>776500</v>
       </c>
       <c r="S2" s="13">
         <f>U2-R2</f>
-        <v>1000</v>
+        <v>3500</v>
       </c>
       <c r="T2" s="11">
         <f>na1_*ra1_+na2_*ra2_+na3_*ra3_</f>
@@ -854,7 +854,7 @@
       </c>
       <c r="U2" s="11">
         <f>nc1_*mc1_+nc2_*mc2_+nc3_*mc3_</f>
-        <v>781000</v>
+        <v>780000</v>
       </c>
       <c r="V2" s="11">
         <f>nc1_*I6+nc2_*I7+nc3_*I8</f>
@@ -866,7 +866,7 @@
       </c>
       <c r="X2" s="11">
         <f>nc1_*rc_1+nc2_*rc_2+nc3_*rc_3</f>
-        <v>21000</v>
+        <v>21010</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -997,7 +997,7 @@
       </c>
       <c r="I5" s="1">
         <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na3_)*M5)+L5</f>
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J5" s="20" t="str">
         <f t="shared" si="0"/>
@@ -1036,26 +1036,25 @@
         <v>10</v>
       </c>
       <c r="E6" s="14">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc1_)*G6)</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G6" s="22">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H6" s="14">
-        <f>100+K6</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc1_)*M6)+L6</f>
-        <v>780</v>
+        <v>0</v>
       </c>
       <c r="J6" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Messages must be 0 on 0 Relationships</v>
       </c>
       <c r="K6" s="19">
         <v>0</v>
@@ -1064,7 +1063,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="24">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="N6" s="14">
         <v>0</v>
@@ -1094,10 +1093,10 @@
       </c>
       <c r="F7" s="2">
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc2_)*G7)</f>
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="G7" s="23">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="H7" s="14">
         <f>12000+K7</f>
@@ -1105,7 +1104,7 @@
       </c>
       <c r="I7" s="1">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc2_)*M7)+L7</f>
-        <v>9360</v>
+        <v>9750</v>
       </c>
       <c r="J7" s="20" t="str">
         <f t="shared" si="0"/>
@@ -1118,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="24">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="N7" s="14">
         <v>0</v>
@@ -1750,7 +1749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E26EECF-D978-410A-A017-B2DC302577D6}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>

</xml_diff>

<commit_message>
fix: PR review refactorings
</commit_message>
<xml_diff>
--- a/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData-plusNewMedium.xlsx
+++ b/Applications/ConsumerApi/test/ConsumerApi.Tests.Performance.SnapshotCreator.Tests/TestData/PerformanceTestData-plusNewMedium.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev-js\backbone\Applications\ConsumerApi\test\ConsumerApi.Tests.Performance.SnapshotCreator.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2507222C-6902-400D-9D53-8E556D7558DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04292F75-ECBA-446B-9DE1-67C6778F887B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="270" windowWidth="28740" windowHeight="14580" tabRatio="259" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="33225" windowHeight="7095" tabRatio="259" xr2:uid="{92C40C20-5DD5-42C1-8294-9AF7E00B4BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="heavy" sheetId="1" r:id="rId1"/>
@@ -263,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +293,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -310,10 +316,6 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -340,7 +342,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -352,6 +353,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -369,6 +375,202 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1382512</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0418D8CF-B4DE-E453-3784-156F8C4A4A31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="582706" y="1916206"/>
+          <a:ext cx="6828571" cy="2019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1382512</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6344E836-CC0E-FA8C-2A4C-080F514FCD39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="582706" y="1916206"/>
+          <a:ext cx="6828571" cy="2019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1382512</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D4664ED-8335-7B51-9470-85948F946BB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="582706" y="1916206"/>
+          <a:ext cx="6828571" cy="2019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>878248</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E56467C-C60B-2A19-7EB7-37B4ED6B58DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="672353" y="1916206"/>
+          <a:ext cx="6828571" cy="2019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -692,7 +894,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,495 +926,495 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
         <v>5000</v>
       </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14">
+      <c r="E2" s="12">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12">
         <v>50</v>
       </c>
-      <c r="O2" s="14">
-        <v>1</v>
-      </c>
-      <c r="P2" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="11">
+      <c r="O2" s="12">
+        <v>1</v>
+      </c>
+      <c r="P2" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="9">
         <f>na1_*ma1_+na2_*ma2_+na3_*ma3_</f>
-        <v>780000</v>
-      </c>
-      <c r="R2" s="11">
+        <v>775000</v>
+      </c>
+      <c r="R2" s="9">
         <f>na1_*I3+na2_*I4+na3_*I5</f>
-        <v>776500</v>
-      </c>
-      <c r="S2" s="13">
+        <v>779500</v>
+      </c>
+      <c r="S2" s="11">
         <f>U2-R2</f>
-        <v>3500</v>
-      </c>
-      <c r="T2" s="11">
+        <v>500</v>
+      </c>
+      <c r="T2" s="9">
         <f>na1_*ra1_+na2_*ra2_+na3_*ra3_</f>
-        <v>21000</v>
-      </c>
-      <c r="U2" s="11">
+        <v>20500</v>
+      </c>
+      <c r="U2" s="9">
         <f>nc1_*mc1_+nc2_*mc2_+nc3_*mc3_</f>
         <v>780000</v>
       </c>
-      <c r="V2" s="11">
+      <c r="V2" s="9">
         <f>nc1_*I6+nc2_*I7+nc3_*I8</f>
-        <v>780000</v>
-      </c>
-      <c r="W2" s="13">
+        <v>774990</v>
+      </c>
+      <c r="W2" s="11">
         <f>Q2-V2</f>
-        <v>0</v>
-      </c>
-      <c r="X2" s="11">
+        <v>10</v>
+      </c>
+      <c r="X2" s="9">
         <f>nc1_*rc_1+nc2_*rc_2+nc3_*rc_3</f>
-        <v>21010</v>
+        <v>20530</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <v>500</v>
       </c>
-      <c r="E3" s="14">
-        <v>1</v>
-      </c>
-      <c r="F3" s="14">
-        <v>1</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14">
-        <f>10+K3</f>
-        <v>10</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="23">
         <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na1_)*M3)+L3</f>
-        <v>15</v>
-      </c>
-      <c r="J3" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="J3" s="17" t="str">
         <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
-        <v/>
-      </c>
-      <c r="K3" s="19">
-        <v>0</v>
-      </c>
-      <c r="L3" s="19">
-        <v>0</v>
-      </c>
-      <c r="M3" s="24">
-        <v>0.01</v>
-      </c>
-      <c r="N3" s="14">
+        <v>Messages must be 0 on 0 Relationships</v>
+      </c>
+      <c r="K3" s="24">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24">
+        <v>0</v>
+      </c>
+      <c r="M3" s="21">
+        <v>0</v>
+      </c>
+      <c r="N3" s="12">
         <v>50</v>
       </c>
-      <c r="O3" s="14">
-        <v>1</v>
-      </c>
-      <c r="P3" s="15">
+      <c r="O3" s="12">
+        <v>1</v>
+      </c>
+      <c r="P3" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>1500</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>2</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="12">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14">
+      <c r="G4" s="12"/>
+      <c r="H4" s="12">
         <f>50+K4</f>
         <v>50</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="23">
         <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na2_)*M4)+L4</f>
         <v>130</v>
       </c>
-      <c r="J4" s="20" t="str">
+      <c r="J4" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="19">
-        <v>0</v>
-      </c>
-      <c r="L4" s="19">
-        <v>0</v>
-      </c>
-      <c r="M4" s="24">
+      <c r="K4" s="24">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24">
+        <v>0</v>
+      </c>
+      <c r="M4" s="21">
         <v>0.25</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="12">
         <v>500</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="12">
         <v>2</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>3500</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>5</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>5</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="G5" s="12"/>
+      <c r="H5" s="12">
         <f>200+K5</f>
         <v>200</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="23">
         <f>_xlfn.FLOOR.MATH((nc1_*mc1_+mc2_*nc2_+mc3_*nc3_)/(na3_)*M5)+L5</f>
-        <v>164</v>
-      </c>
-      <c r="J5" s="20" t="str">
+        <v>167</v>
+      </c>
+      <c r="J5" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="19">
-        <v>0</v>
-      </c>
-      <c r="L5" s="19">
-        <v>0</v>
-      </c>
-      <c r="M5" s="24">
-        <v>0.74</v>
-      </c>
-      <c r="N5" s="14">
+      <c r="K5" s="24">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="N5" s="12">
         <v>1500</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="12">
         <v>3</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>10</v>
       </c>
-      <c r="E6" s="14">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="23">
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc1_)*G6)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="22">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="G6" s="19">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="23">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc1_)*M6)+L6</f>
         <v>0</v>
       </c>
-      <c r="J6" s="20" t="str">
+      <c r="J6" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Messages must be 0 on 0 Relationships</v>
       </c>
-      <c r="K6" s="19">
-        <v>0</v>
-      </c>
-      <c r="L6" s="19">
-        <v>0</v>
-      </c>
-      <c r="M6" s="24">
-        <v>0</v>
-      </c>
-      <c r="N6" s="14">
-        <v>0</v>
-      </c>
-      <c r="O6" s="14">
-        <v>1</v>
-      </c>
-      <c r="P6" s="15">
+      <c r="K6" s="24">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
+        <v>0</v>
+      </c>
+      <c r="M6" s="21">
+        <v>0</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
+        <v>1</v>
+      </c>
+      <c r="P6" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>20</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>8000</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="22">
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc2_)*G7)</f>
-        <v>263</v>
-      </c>
-      <c r="G7" s="23">
+        <v>257</v>
+      </c>
+      <c r="G7" s="20">
         <v>0.25</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <f>12000+K7</f>
         <v>12000</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="23">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc2_)*M7)+L7</f>
-        <v>9750</v>
-      </c>
-      <c r="J7" s="20" t="str">
+        <v>9687</v>
+      </c>
+      <c r="J7" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="19">
-        <v>0</v>
-      </c>
-      <c r="L7" s="19">
-        <v>0</v>
-      </c>
-      <c r="M7" s="24">
+      <c r="K7" s="24">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
         <v>0.25</v>
       </c>
-      <c r="N7" s="14">
-        <v>0</v>
-      </c>
-      <c r="O7" s="14">
-        <v>1</v>
-      </c>
-      <c r="P7" s="15">
+      <c r="N7" s="12">
+        <v>0</v>
+      </c>
+      <c r="O7" s="12">
+        <v>1</v>
+      </c>
+      <c r="P7" s="13">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>30</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>12000</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="22">
         <f>_xlfn.CEILING.MATH((na1_*ra1_+na2_*ra2_+na3_*ra3_)/(nc3_)*G8)</f>
-        <v>525</v>
-      </c>
-      <c r="G8" s="23">
+        <v>513</v>
+      </c>
+      <c r="G8" s="20">
         <v>0.75</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <f>18000+K8</f>
         <v>18000</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="23">
         <f>_xlfn.FLOOR.MATH((na1_*ma1_+ma2_*na2_+ma3_*na3_)/(nc3_)*M8)+L8</f>
-        <v>19500</v>
-      </c>
-      <c r="J8" s="20" t="str">
+        <v>19375</v>
+      </c>
+      <c r="J8" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="19">
-        <v>0</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0</v>
-      </c>
-      <c r="M8" s="24">
+      <c r="K8" s="24">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+      <c r="M8" s="21">
         <v>0.75</v>
       </c>
-      <c r="N8" s="14">
-        <v>0</v>
-      </c>
-      <c r="O8" s="14">
-        <v>1</v>
-      </c>
-      <c r="P8" s="15">
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <v>1</v>
+      </c>
+      <c r="P8" s="13">
         <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1223,7 +1425,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1447,7 @@
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.42578125" customWidth="1"/>
     <col min="19" max="19" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="37.42578125" bestFit="1" customWidth="1"/>
@@ -1255,493 +1457,494 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
         <v>2500</v>
       </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14">
+      <c r="E2" s="12">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12">
         <v>25</v>
       </c>
-      <c r="O2" s="14">
-        <v>1</v>
-      </c>
-      <c r="P2" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="11">
+      <c r="O2" s="12">
+        <v>1</v>
+      </c>
+      <c r="P2" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="9">
         <f>D3*H3+D4*H4+D5*H5</f>
         <v>195000</v>
       </c>
-      <c r="R2" s="16">
+      <c r="R2" s="14">
         <f>D3*I3+D4*I4+D5*I5</f>
         <v>194000</v>
       </c>
-      <c r="S2" s="17">
+      <c r="S2" s="15">
         <f>U2-R2</f>
         <v>1250</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="9">
         <f>D3*F3+D4*F4+D5*F5</f>
         <v>4500</v>
       </c>
-      <c r="U2" s="11">
+      <c r="U2" s="9">
         <f>D6*H6+D7*H7+D8*H8</f>
         <v>195250</v>
       </c>
-      <c r="V2" s="16">
+      <c r="V2" s="14">
         <f>D6*I6+D7*I7+D8*I8</f>
         <v>195000</v>
       </c>
-      <c r="W2" s="13">
+      <c r="W2" s="11">
         <f>Q2-V2</f>
         <v>0</v>
       </c>
-      <c r="X2" s="11">
+      <c r="X2" s="9">
         <f>D6*F6+D7*F7+D8*F8</f>
         <v>4500</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <v>250</v>
       </c>
-      <c r="E3" s="14">
-        <v>1</v>
-      </c>
-      <c r="F3" s="14">
-        <v>1</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14">
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12">
         <v>5</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="23">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D3)*M3)+L3</f>
         <v>7</v>
       </c>
-      <c r="J3" s="20" t="str">
+      <c r="J3" s="17" t="str">
         <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
         <v/>
       </c>
-      <c r="K3" s="19">
-        <v>0</v>
-      </c>
-      <c r="L3" s="19">
-        <v>0</v>
-      </c>
-      <c r="M3" s="24">
+      <c r="K3" s="24">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24">
+        <v>0</v>
+      </c>
+      <c r="M3" s="21">
         <v>0.01</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="12">
         <v>25</v>
       </c>
-      <c r="O3" s="14">
-        <v>1</v>
-      </c>
-      <c r="P3" s="15">
+      <c r="O3" s="12">
+        <v>1</v>
+      </c>
+      <c r="P3" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>750</v>
       </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="14">
-        <v>1</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14">
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12">
         <v>25</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="23">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D4)*M4)+L4</f>
         <v>65</v>
       </c>
-      <c r="J4" s="20" t="str">
+      <c r="J4" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="19">
-        <v>0</v>
-      </c>
-      <c r="L4" s="19">
-        <v>0</v>
-      </c>
-      <c r="M4" s="24">
+      <c r="K4" s="24">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24">
+        <v>0</v>
+      </c>
+      <c r="M4" s="21">
         <v>0.25</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="12">
         <v>250</v>
       </c>
-      <c r="O4" s="14">
-        <v>1</v>
-      </c>
-      <c r="P4" s="15">
+      <c r="O4" s="12">
+        <v>1</v>
+      </c>
+      <c r="P4" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>1750</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>2</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>2</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="G5" s="12"/>
+      <c r="H5" s="12">
         <v>100</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="23">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D5)*M5)+L5</f>
         <v>82</v>
       </c>
-      <c r="J5" s="20" t="str">
+      <c r="J5" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="19">
-        <v>0</v>
-      </c>
-      <c r="L5" s="19">
-        <v>0</v>
-      </c>
-      <c r="M5" s="24">
+      <c r="K5" s="24">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21">
         <v>0.74</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="12">
         <v>750</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="12">
         <v>2</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>5</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
         <v>50</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="22">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*G6)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="19">
         <v>0.01</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="12">
         <v>50</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="23">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D6)*M6)+L6</f>
         <v>390</v>
       </c>
-      <c r="J6" s="20" t="str">
+      <c r="J6" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K6" s="19">
-        <v>0</v>
-      </c>
-      <c r="L6" s="19">
-        <v>0</v>
-      </c>
-      <c r="M6" s="24">
+      <c r="K6" s="24">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
+        <v>0</v>
+      </c>
+      <c r="M6" s="21">
         <v>0.01</v>
       </c>
-      <c r="N6" s="14">
-        <v>0</v>
-      </c>
-      <c r="O6" s="14">
-        <v>1</v>
-      </c>
-      <c r="P6" s="15">
+      <c r="N6" s="12">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
+        <v>1</v>
+      </c>
+      <c r="P6" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>10</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>4000</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="22">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*G7)</f>
         <v>108</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="19">
         <v>0.24</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <v>6000</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="23">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D7)*M7)+L7</f>
         <v>4680</v>
       </c>
-      <c r="J7" s="20" t="str">
+      <c r="J7" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="19">
-        <v>0</v>
-      </c>
-      <c r="L7" s="19">
-        <v>0</v>
-      </c>
-      <c r="M7" s="24">
+      <c r="K7" s="24">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
         <v>0.24</v>
       </c>
-      <c r="N7" s="14">
-        <v>0</v>
-      </c>
-      <c r="O7" s="14">
-        <v>1</v>
-      </c>
-      <c r="P7" s="15">
+      <c r="N7" s="12">
+        <v>0</v>
+      </c>
+      <c r="O7" s="12">
+        <v>1</v>
+      </c>
+      <c r="P7" s="13">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>15</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>6000</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="22">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*G8)</f>
         <v>225</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="19">
         <v>0.75</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <v>9000</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="23">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D8)*M8)+L8</f>
         <v>9750</v>
       </c>
-      <c r="J8" s="20" t="str">
+      <c r="J8" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="19">
-        <v>0</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0</v>
-      </c>
-      <c r="M8" s="24">
+      <c r="K8" s="24">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+      <c r="M8" s="21">
         <v>0.75</v>
       </c>
-      <c r="N8" s="14">
-        <v>0</v>
-      </c>
-      <c r="O8" s="14">
-        <v>1</v>
-      </c>
-      <c r="P8" s="15">
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <v>1</v>
+      </c>
+      <c r="P8" s="13">
         <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="18"/>
+      <c r="F11" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1752,7 +1955,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1977,7 @@
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.7109375" customWidth="1"/>
     <col min="19" max="19" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="37.42578125" bestFit="1" customWidth="1"/>
@@ -1784,499 +1987,500 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
         <v>10</v>
       </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14">
+      <c r="E2" s="12">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12">
         <v>50</v>
       </c>
-      <c r="O2" s="14">
-        <v>1</v>
-      </c>
-      <c r="P2" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="11">
+      <c r="O2" s="12">
+        <v>1</v>
+      </c>
+      <c r="P2" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="9">
         <f>D3*H3+D4*H4+D5*H5</f>
         <v>16500</v>
       </c>
-      <c r="R2" s="16">
+      <c r="R2" s="14">
         <f>D3*I3+D4*I4+D5*I5</f>
-        <v>16500</v>
-      </c>
-      <c r="S2" s="17">
+        <v>16800</v>
+      </c>
+      <c r="S2" s="15">
         <f>U2-R2</f>
-        <v>0</v>
-      </c>
-      <c r="T2" s="11">
+        <v>-300</v>
+      </c>
+      <c r="T2" s="9">
         <f>D3*F3+D4*F4+D5*F5</f>
         <v>1800</v>
       </c>
-      <c r="U2" s="11">
+      <c r="U2" s="9">
         <f>D6*H6+D7*H7+D8*H8</f>
         <v>16500</v>
       </c>
-      <c r="V2" s="16">
+      <c r="V2" s="14">
         <f>D6*I6+D7*I7+D8*I8</f>
         <v>16499</v>
       </c>
-      <c r="W2" s="13">
+      <c r="W2" s="11">
         <f>Q2-V2</f>
         <v>1</v>
       </c>
-      <c r="X2" s="11">
+      <c r="X2" s="9">
         <f>D6*F6+D7*F7+D8*F8</f>
         <v>1803</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="12">
         <v>50</v>
       </c>
-      <c r="E3" s="14">
-        <v>0</v>
-      </c>
-      <c r="F3" s="14">
-        <v>0</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14">
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12">
         <f>0+K3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="23">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D3)*M3)+L3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="20" t="str">
+      <c r="J3" s="17" t="str">
         <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
         <v>Messages must be 0 on 0 Relationships</v>
       </c>
-      <c r="K3" s="19">
-        <v>0</v>
-      </c>
-      <c r="L3" s="19">
-        <v>-3</v>
-      </c>
-      <c r="M3" s="24">
-        <v>0.01</v>
-      </c>
-      <c r="N3" s="14">
+      <c r="K3" s="24">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24">
+        <v>0</v>
+      </c>
+      <c r="M3" s="21">
+        <v>0</v>
+      </c>
+      <c r="N3" s="12">
         <v>5</v>
       </c>
-      <c r="O3" s="14">
-        <v>1</v>
-      </c>
-      <c r="P3" s="15">
+      <c r="O3" s="12">
+        <v>1</v>
+      </c>
+      <c r="P3" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>150</v>
       </c>
-      <c r="E4" s="14">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14">
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14">
+      <c r="G4" s="12"/>
+      <c r="H4" s="12">
         <f>10+K4</f>
         <v>10</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="23">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D4)*M4)+L4</f>
         <v>30</v>
       </c>
-      <c r="J4" s="20" t="str">
+      <c r="J4" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="19">
-        <v>0</v>
-      </c>
-      <c r="L4" s="19">
+      <c r="K4" s="24">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24">
         <v>3</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="21">
         <v>0.25</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="12">
         <v>60</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="12">
         <v>2</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>300</v>
       </c>
-      <c r="E5" s="14">
-        <v>0</v>
-      </c>
-      <c r="F5" s="14">
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
         <v>5</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="G5" s="12"/>
+      <c r="H5" s="12">
         <f>50+K5</f>
         <v>50</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="23">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D5)*M5)+L5</f>
-        <v>40</v>
-      </c>
-      <c r="J5" s="20" t="str">
+        <v>41</v>
+      </c>
+      <c r="J5" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="19">
-        <v>0</v>
-      </c>
-      <c r="L5" s="19">
-        <v>0</v>
-      </c>
-      <c r="M5" s="24">
-        <v>0.74</v>
-      </c>
-      <c r="N5" s="14">
-        <v>1</v>
-      </c>
-      <c r="O5" s="14">
+      <c r="K5" s="24">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="N5" s="12">
+        <v>1</v>
+      </c>
+      <c r="O5" s="12">
         <v>3</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6" s="14">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="22">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*G6)</f>
         <v>9</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="19">
         <v>0.01</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="12">
         <f>0+K6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="23">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D6)*M6)+L6</f>
         <v>82</v>
       </c>
-      <c r="J6" s="20" t="str">
+      <c r="J6" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K6" s="19">
-        <v>0</v>
-      </c>
-      <c r="L6" s="19">
-        <v>0</v>
-      </c>
-      <c r="M6" s="24">
+      <c r="K6" s="24">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
+        <v>0</v>
+      </c>
+      <c r="M6" s="21">
         <v>0.01</v>
       </c>
-      <c r="N6" s="14">
-        <v>0</v>
-      </c>
-      <c r="O6" s="14">
-        <v>1</v>
-      </c>
-      <c r="P6" s="15">
+      <c r="N6" s="12">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
+        <v>1</v>
+      </c>
+      <c r="P6" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>15</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>20</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="22">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*G7)</f>
         <v>29</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="19">
         <v>0.24</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <f>440+K7</f>
         <v>440</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="23">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D7)*M7)+L7</f>
         <v>264</v>
       </c>
-      <c r="J7" s="20" t="str">
+      <c r="J7" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="19">
-        <v>0</v>
-      </c>
-      <c r="L7" s="19">
-        <v>0</v>
-      </c>
-      <c r="M7" s="24">
+      <c r="K7" s="24">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
         <v>0.24</v>
       </c>
-      <c r="N7" s="14">
-        <v>0</v>
-      </c>
-      <c r="O7" s="14">
-        <v>1</v>
-      </c>
-      <c r="P7" s="15">
+      <c r="N7" s="12">
+        <v>0</v>
+      </c>
+      <c r="O7" s="12">
+        <v>1</v>
+      </c>
+      <c r="P7" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>15</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>30</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="22">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*G8)</f>
         <v>90</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="19">
         <v>0.75</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <f>660+K8</f>
         <v>660</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="23">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D8)*M8)+L8</f>
         <v>825</v>
       </c>
-      <c r="J8" s="20" t="str">
+      <c r="J8" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="19">
-        <v>0</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0</v>
-      </c>
-      <c r="M8" s="24">
+      <c r="K8" s="24">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+      <c r="M8" s="21">
         <v>0.75</v>
       </c>
-      <c r="N8" s="14">
-        <v>0</v>
-      </c>
-      <c r="O8" s="14">
-        <v>1</v>
-      </c>
-      <c r="P8" s="15">
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <v>1</v>
+      </c>
+      <c r="P8" s="13">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="18"/>
+      <c r="F11" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2284,9 +2488,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7916CF-DA95-4AEE-886B-16E22DB90DBC}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,496 +2522,497 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
         <v>5</v>
       </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="14">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="14">
+      <c r="E2" s="12">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="12">
         <v>50</v>
       </c>
-      <c r="O2" s="14">
-        <v>1</v>
-      </c>
-      <c r="P2" s="15">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="11">
+      <c r="O2" s="12">
+        <v>1</v>
+      </c>
+      <c r="P2" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="9">
         <f>D3*H3+D4*H4+D5*H5</f>
         <v>48</v>
       </c>
-      <c r="R2" s="16">
+      <c r="R2" s="14">
         <f>D3*I3+D4*I4+D5*I5</f>
         <v>45</v>
       </c>
-      <c r="S2" s="17">
+      <c r="S2" s="15">
         <f>U2-R2</f>
         <v>3</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="9">
         <f>D3*F3+D4*F4+D5*F5</f>
         <v>22</v>
       </c>
-      <c r="U2" s="11">
+      <c r="U2" s="9">
         <f>D6*H6+D7*H7+D8*H8</f>
         <v>48</v>
       </c>
-      <c r="V2" s="16">
+      <c r="V2" s="14">
         <f>D6*I6+D7*I7+D8*I8</f>
         <v>46</v>
       </c>
-      <c r="W2" s="13">
+      <c r="W2" s="11">
         <f>Q2-V2</f>
         <v>2</v>
       </c>
-      <c r="X2" s="11">
+      <c r="X2" s="9">
         <f>D6*F6+D7*F7+D8*F8</f>
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14">
-        <v>1</v>
-      </c>
-      <c r="E3" s="14">
-        <v>0</v>
-      </c>
-      <c r="F3" s="14">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="14">
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="12">
         <f>0+K3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="23">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D3)*M3)+L3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="20" t="str">
+      <c r="J3" s="17" t="str">
         <f t="shared" ref="J3:J8" si="0">IF(F3=0, "Messages must be 0 on 0 Relationships", "")</f>
         <v/>
       </c>
-      <c r="K3" s="19">
-        <v>0</v>
-      </c>
-      <c r="L3" s="19">
-        <v>0</v>
-      </c>
-      <c r="M3" s="7">
+      <c r="K3" s="24">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
         <v>0.01</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="12">
         <v>50</v>
       </c>
-      <c r="O3" s="14">
-        <v>1</v>
-      </c>
-      <c r="P3" s="15">
+      <c r="O3" s="12">
+        <v>1</v>
+      </c>
+      <c r="P3" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>3</v>
       </c>
-      <c r="E4" s="14">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14">
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
         <v>2</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="14">
+      <c r="G4" s="3"/>
+      <c r="H4" s="12">
         <f>4+K4</f>
         <v>4</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="23">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D4)*M4)+L4</f>
         <v>4</v>
       </c>
-      <c r="J4" s="20" t="str">
+      <c r="J4" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="19">
-        <v>0</v>
-      </c>
-      <c r="L4" s="19">
-        <v>0</v>
-      </c>
-      <c r="M4" s="7">
+      <c r="K4" s="24">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
         <v>0.25</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="12">
         <v>60</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="12">
         <v>2</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>3</v>
       </c>
-      <c r="E5" s="14">
-        <v>0</v>
-      </c>
-      <c r="F5" s="14">
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
         <v>5</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="14">
+      <c r="G5" s="3"/>
+      <c r="H5" s="12">
         <f>12+K5</f>
         <v>12</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="23">
         <f>_xlfn.FLOOR.MATH((D6*H6+D7*H7+D8*H8)/(D5)*M5)+L5</f>
         <v>11</v>
       </c>
-      <c r="J5" s="20" t="str">
+      <c r="J5" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K5" s="19">
-        <v>0</v>
-      </c>
-      <c r="L5" s="19">
-        <v>0</v>
-      </c>
-      <c r="M5" s="7">
+      <c r="K5" s="24">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
         <v>0.74</v>
       </c>
-      <c r="N5" s="14">
-        <v>1</v>
-      </c>
-      <c r="O5" s="14">
+      <c r="N5" s="12">
+        <v>1</v>
+      </c>
+      <c r="O5" s="12">
         <v>3</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14">
-        <v>1</v>
-      </c>
-      <c r="E6" s="14">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="22">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D6)*G6)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <v>0.01</v>
       </c>
-      <c r="H6" s="14">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="23">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D6)*M6)+L6</f>
         <v>0</v>
       </c>
-      <c r="J6" s="20" t="str">
+      <c r="J6" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K6" s="19">
-        <v>0</v>
-      </c>
-      <c r="L6" s="19">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7">
+      <c r="K6" s="24">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
         <v>0.01</v>
       </c>
-      <c r="N6" s="14">
-        <v>0</v>
-      </c>
-      <c r="O6" s="14">
-        <v>1</v>
-      </c>
-      <c r="P6" s="15">
+      <c r="N6" s="12">
+        <v>0</v>
+      </c>
+      <c r="O6" s="12">
+        <v>1</v>
+      </c>
+      <c r="P6" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>2</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>20</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="22">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D7)*G7)</f>
         <v>3</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="10">
         <v>0.24</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <f>8+K7</f>
         <v>8</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="23">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D7)*M7)+L7</f>
         <v>5</v>
       </c>
-      <c r="J7" s="20" t="str">
+      <c r="J7" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K7" s="19">
-        <v>0</v>
-      </c>
-      <c r="L7" s="19">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7">
+      <c r="K7" s="24">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
         <v>0.24</v>
       </c>
-      <c r="N7" s="14">
-        <v>0</v>
-      </c>
-      <c r="O7" s="14">
-        <v>1</v>
-      </c>
-      <c r="P7" s="15">
+      <c r="N7" s="12">
+        <v>0</v>
+      </c>
+      <c r="O7" s="12">
+        <v>1</v>
+      </c>
+      <c r="P7" s="13">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>4</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>30</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="22">
         <f>_xlfn.CEILING.MATH((D3*F3+D4*F4+D5*F5)/(D8)*G8)</f>
         <v>5</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <v>0.75</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <f>8+K8</f>
         <v>8</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="23">
         <f>_xlfn.FLOOR.MATH((D3*H3+D4*H4+D5*H5)/(D8)*M8)+L8</f>
         <v>9</v>
       </c>
-      <c r="J8" s="20" t="str">
+      <c r="J8" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K8" s="19">
-        <v>0</v>
-      </c>
-      <c r="L8" s="19">
-        <v>0</v>
-      </c>
-      <c r="M8" s="7">
+      <c r="K8" s="24">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
         <v>0.75</v>
       </c>
-      <c r="N8" s="14">
-        <v>0</v>
-      </c>
-      <c r="O8" s="14">
-        <v>1</v>
-      </c>
-      <c r="P8" s="15">
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+      <c r="O8" s="12">
+        <v>1</v>
+      </c>
+      <c r="P8" s="13">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="18"/>
+      <c r="F11" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>